<commit_message>
feat: Actualizacion de programa y archivos para cargue
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{232F4A63-288E-44E8-B430-9BC74527BEAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41E0072-0810-4565-AA3A-D2AFD7E8663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,382 +437,82 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>9</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>4</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>5</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>12</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>12</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
         <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevas celdas agregadas en el archivo mines.csv
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41E0072-0810-4565-AA3A-D2AFD7E8663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A0E00F-DC92-4483-954A-E6B40BE0FEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,80 +439,748 @@
       <c r="A2">
         <v>13</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>13</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>14</v>
       </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>14</v>
       </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>15</v>
       </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>15</v>
       </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>15</v>
       </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>16</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>18</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>19</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>5</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>21</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>21</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>21</v>
+      </c>
+      <c r="B36">
+        <v>5</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>21</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>22</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>22</v>
+      </c>
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>22</v>
+      </c>
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>22</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>23</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>23</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>24</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>24</v>
+      </c>
+      <c r="B49">
+        <v>5</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>25</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>25</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>25</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>25</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>26</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>26</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>26</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>26</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+      <c r="C57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>27</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>27</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>27</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>27</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>28</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>28</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>28</v>
+      </c>
+      <c r="B64">
+        <v>3</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>28</v>
+      </c>
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>29</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>29</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>29</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>29</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambio del codigo para invertir la lectura de las minas
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A0E00F-DC92-4483-954A-E6B40BE0FEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8520161F-23A8-40F1-8A56-C723FEB3FF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
@@ -418,8 +418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,10 +429,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nueva version de cambios
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferch\OneDrive\Documentos\GitHub\detect_mines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845739C6-F45A-4B44-B440-FAC5ABF636FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208D9E6B-FA20-4D1C-A1E9-E3BF1A6373A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -416,13 +416,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="88.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -437,76 +440,76 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -514,51 +517,51 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -569,7 +572,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -580,109 +583,109 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>4</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B21">
         <v>5</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C24">
         <v>4</v>
@@ -690,21 +693,21 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -712,210 +715,78 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
         <v>5</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B32">
         <v>4</v>
       </c>
       <c r="C32">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B33">
         <v>5</v>
       </c>
       <c r="C33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>38</v>
-      </c>
-      <c r="B34">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>38</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>38</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>38</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>39</v>
-      </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-      <c r="C38">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>39</v>
-      </c>
-      <c r="B39">
-        <v>2</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-      <c r="C42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>40</v>
-      </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-      <c r="C43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>40</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>40</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nueva version del programa establecido para almacenar archivos csv y crear las imagnes de los heat maps
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56919DDA-5BCB-4F2A-877F-CC6772A258D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8E4607-E575-4CA0-93D1-B99C90DB6D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5865" yWindow="630" windowWidth="5580" windowHeight="6585" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -416,16 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="N8" activeCellId="1" sqref="L7 N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="88.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -440,46 +437,178 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>1</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>5</v>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
nuevos registros de juegos
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8E4607-E575-4CA0-93D1-B99C90DB6D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0038B2F-B943-4DA6-83D2-CBBC8C913A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
+    <workbookView xWindow="420" yWindow="1275" windowWidth="5145" windowHeight="8325" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" activeCellId="1" sqref="L7 N8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,178 +437,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
         <v>5</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>8</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>5</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios nuevos en md y excel
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usar2\OneDrive - uniminuto.edu\Documentos\GitHub\detect_mines\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0038B2F-B943-4DA6-83D2-CBBC8C913A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C241132F-AB91-4F2C-A57E-9866B1B197B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="1275" windowWidth="5145" windowHeight="8325" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
+    <workbookView xWindow="1140" yWindow="2385" windowWidth="6345" windowHeight="11175" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -437,35 +437,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>4</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambio en el codigo fuente del generador de csv y graficas
</commit_message>
<xml_diff>
--- a/partidas_mines.xlsx
+++ b/partidas_mines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\GitHub\detect_mines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C241132F-AB91-4F2C-A57E-9866B1B197B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC918E0D-B688-472B-8CC4-631A26FD9C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2385" windowWidth="6345" windowHeight="11175" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
+    <workbookView xWindow="-15300" yWindow="520" windowWidth="5940" windowHeight="7360" xr2:uid="{28234BB7-34D6-40F0-9F81-F11149BF6DC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>partida</t>
   </si>
@@ -46,15 +46,24 @@
   <si>
     <t>columna</t>
   </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B531AC-16A0-4190-833B-D0DCF47D07F9}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,7 +444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -443,32 +452,38 @@
         <v>1</v>
       </c>
       <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>